<commit_message>
add additional supplementary docs for CSSI
</commit_message>
<xml_diff>
--- a/CSSI_2019/forms/CSSI_2019_Budget_AmyRoberts_CA.xlsx
+++ b/CSSI_2019/forms/CSSI_2019_Budget_AmyRoberts_CA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\canto\Repositories\SI2.git\CSSI_2019\forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23BBB21F-4B69-4443-A064-A4C11B07DAED}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87B41C3E-161E-4012-9E92-D14E9D3843D5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -957,8 +957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -1783,17 +1783,20 @@
         <v>21</v>
       </c>
       <c r="B42" s="23">
-        <v>3220</v>
+        <f>3220+1220</f>
+        <v>4440</v>
       </c>
       <c r="C42" s="23">
-        <v>3220</v>
+        <f>3220+1220</f>
+        <v>4440</v>
       </c>
       <c r="D42" s="23">
-        <v>3220</v>
+        <f>3220+1220</f>
+        <v>4440</v>
       </c>
       <c r="E42" s="18">
         <f>SUM(B42:D42)</f>
-        <v>9660</v>
+        <v>13320</v>
       </c>
       <c r="F42" s="26"/>
       <c r="G42" s="26"/>
@@ -1816,19 +1819,19 @@
       </c>
       <c r="B44" s="19">
         <f>SUM(B42:B43)</f>
-        <v>3220</v>
+        <v>4440</v>
       </c>
       <c r="C44" s="19">
         <f>SUM(C42:C43)</f>
-        <v>3220</v>
+        <v>4440</v>
       </c>
       <c r="D44" s="19">
         <f>SUM(D42:D43)</f>
-        <v>3220</v>
+        <v>4440</v>
       </c>
       <c r="E44" s="18">
         <f>SUM(B44:D44)</f>
-        <v>9660</v>
+        <v>13320</v>
       </c>
       <c r="F44" s="29"/>
       <c r="G44" s="29"/>
@@ -1868,14 +1871,14 @@
         <v>2000</v>
       </c>
       <c r="C47" s="9">
-        <v>4000</v>
+        <v>2000</v>
       </c>
       <c r="D47" s="9">
-        <v>4000</v>
+        <v>2000</v>
       </c>
       <c r="E47" s="18">
         <f t="shared" ref="E47:E55" si="8">SUM(B47:D47)</f>
-        <v>10000</v>
+        <v>6000</v>
       </c>
       <c r="F47" s="25"/>
       <c r="K47" t="s">
@@ -1992,15 +1995,15 @@
       </c>
       <c r="C55" s="19">
         <f>SUM(C47:C54)</f>
-        <v>7185</v>
+        <v>5185</v>
       </c>
       <c r="D55" s="19">
         <f>SUM(D47:D54)</f>
-        <v>7443.5</v>
+        <v>5443.5</v>
       </c>
       <c r="E55" s="18">
         <f t="shared" si="8"/>
-        <v>19578.5</v>
+        <v>15578.5</v>
       </c>
       <c r="F55" s="27"/>
     </row>
@@ -2271,19 +2274,19 @@
       </c>
       <c r="B71" s="18">
         <f>B11+B25+B37+B44+B55-B51</f>
-        <v>104622.82488888889</v>
+        <v>105842.82488888889</v>
       </c>
       <c r="C71" s="18">
         <f>C11+C25+C37+C44+C55-C51</f>
-        <v>109751.40963555555</v>
+        <v>108971.40963555555</v>
       </c>
       <c r="D71" s="18">
         <f>D11+D25+D37+D44+D55-D51</f>
-        <v>122472.81199430223</v>
+        <v>121692.81199430223</v>
       </c>
       <c r="E71" s="18">
         <f>SUM(B71:D71)</f>
-        <v>336847.04651874665</v>
+        <v>336507.04651874665</v>
       </c>
       <c r="F71" s="25"/>
       <c r="G71" s="25"/>
@@ -2308,19 +2311,19 @@
       </c>
       <c r="B73" s="18">
         <f>B11+B25+B37+B44+B55+B69</f>
-        <v>137185.10488888889</v>
+        <v>138405.10488888889</v>
       </c>
       <c r="C73" s="18">
         <f>C11+C25+C37+C44+C55+C69</f>
-        <v>130599.47803555556</v>
+        <v>129819.47803555556</v>
       </c>
       <c r="D73" s="18">
         <f>D11+D25+D37+D44+D55+D69</f>
-        <v>143834.31444630225</v>
+        <v>143054.31444630225</v>
       </c>
       <c r="E73" s="18">
         <f>SUM(B73:D73)</f>
-        <v>411618.89737074671</v>
+        <v>411278.89737074671</v>
       </c>
       <c r="F73" s="25"/>
       <c r="G73" s="25"/>
@@ -2344,19 +2347,19 @@
       </c>
       <c r="B75" s="18">
         <f>B71*0.555</f>
-        <v>58065.667813333341</v>
+        <v>58742.767813333339</v>
       </c>
       <c r="C75" s="18">
         <f>C71*55.5%</f>
-        <v>60912.032347733337</v>
+        <v>60479.132347733335</v>
       </c>
       <c r="D75" s="18">
         <f>D71*55.5%</f>
-        <v>67972.410656837747</v>
+        <v>67539.510656837738</v>
       </c>
       <c r="E75" s="18">
         <f>SUM(B75:D75)</f>
-        <v>186950.11081790441</v>
+        <v>186761.4108179044</v>
       </c>
       <c r="F75" s="24"/>
       <c r="G75" s="24"/>
@@ -2375,19 +2378,19 @@
       </c>
       <c r="B77" s="18">
         <f>B73+B75</f>
-        <v>195250.77270222222</v>
+        <v>197147.87270222223</v>
       </c>
       <c r="C77" s="18">
         <f>C73+C75</f>
-        <v>191511.5103832889</v>
+        <v>190298.61038328888</v>
       </c>
       <c r="D77" s="18">
         <f>D73+D75</f>
-        <v>211806.72510313999</v>
+        <v>210593.82510313997</v>
       </c>
       <c r="E77" s="18">
         <f>SUM(B77:D77)</f>
-        <v>598569.00818865118</v>
+        <v>598040.30818865111</v>
       </c>
       <c r="F77" s="24"/>
       <c r="G77" s="24"/>

</xml_diff>